<commit_message>
CIDC-1594 add urine option
</commit_message>
<xml_diff>
--- a/template_examples/tumor_normal_pairing_template.xlsx
+++ b/template_examples/tumor_normal_pairing_template.xlsx
@@ -244,7 +244,7 @@
     <t xml:space="preserve">Legend for tab 'Tumor-only'</t>
   </si>
   <si>
-    <t xml:space="preserve">Section 'Pair' of tab 'Tumor-only'</t>
+    <t xml:space="preserve">Section 'Tumor-only' of tab 'Tumor-only'</t>
   </si>
 </sst>
 </file>
@@ -493,10 +493,10 @@
   <dimension ref="A1:C2005"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="C1 B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -10570,11 +10570,11 @@
   </sheetPr>
   <dimension ref="A1:C2004"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -10590,7 +10590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
@@ -20686,10 +20686,10 @@
   <dimension ref="B1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -20803,10 +20803,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C1 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>

</xml_diff>